<commit_message>
proyecto terminado y ordenado
</commit_message>
<xml_diff>
--- a/TP_FINAL/Cantidad de Veces de una MAC.xlsx
+++ b/TP_FINAL/Cantidad de Veces de una MAC.xlsx
@@ -456,16 +456,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>30-4B-07-8A-CF-DF</t>
+          <t>48-C7-96-EE-75-1C</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>invitede-pansew</t>
+          <t>csegeview</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>832</v>
+        <v>671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>